<commit_message>
more work for deployment v4
</commit_message>
<xml_diff>
--- a/src/main/resources/sample.xlsx
+++ b/src/main/resources/sample.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>Customer Name:</t>
   </si>
@@ -23,6 +23,9 @@
     <t xml:space="preserve">Customer Account Number: </t>
   </si>
   <si>
+    <t>Invoice Period:</t>
+  </si>
+  <si>
     <t>Invocie Date:</t>
   </si>
   <si>
@@ -32,7 +35,7 @@
     <t>Charges as per Custom Declartion Currency</t>
   </si>
   <si>
-    <t>Charger as per Customer Currency</t>
+    <t>Chargers as per Customer Currency</t>
   </si>
   <si>
     <t>Invoice Type</t>
@@ -77,10 +80,13 @@
     <t>Custom Declartion Currency</t>
   </si>
   <si>
-    <t>Total Amount</t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Invoice Date:</t>
+  </si>
+  <si>
+    <t>Charges as per Customer Currency</t>
   </si>
   <si>
     <t>MAWB</t>
@@ -127,7 +133,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="[$-409]dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -165,11 +171,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -192,7 +193,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border/>
     <border>
       <bottom style="thin">
@@ -249,11 +250,6 @@
       </top>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-    </border>
-    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -276,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -298,6 +294,9 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -309,32 +308,23 @@
     </xf>
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -345,54 +335,41 @@
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="7" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="5" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="8" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="8" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="8" fillId="3" fontId="5" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="8" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="8" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,7 +735,7 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -776,7 +753,7 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -794,172 +771,128 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="9" t="s">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="13" t="s">
+      <c r="B9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="12"/>
     </row>
-    <row r="10" ht="41.25" customHeight="1">
-      <c r="A10" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="16" t="s">
+    <row r="11" ht="41.25" customHeight="1">
+      <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="C11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="D11" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="E11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="F11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="G11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="H11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="I11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="J11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="K11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="L11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="16" t="s">
+      <c r="M11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="O10" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="P10" s="19" t="s">
+      <c r="N11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="Q10" s="19" t="s">
+      <c r="P11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="R10" s="19" t="s">
+      <c r="Q11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="S10" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="14"/>
-      <c r="Z10" s="14"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
+      <c r="R11" s="18" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1"/>
+      <c r="A12" s="19" t="s">
+        <v>22</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
     </row>
     <row r="13" ht="15.75" customHeight="1"/>
     <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="L15" s="25"/>
-    </row>
+    <row r="15" ht="15.75" customHeight="1"/>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
@@ -1946,13 +1879,10 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
-    <row r="1002" ht="15.75" customHeight="1"/>
-    <row r="1003" ht="15.75" customHeight="1"/>
-    <row r="1004" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="O9:R9"/>
+    <mergeCell ref="O10:R10"/>
+    <mergeCell ref="H10:N10"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1996,7 +1926,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2004,135 +1934,129 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
+      <c r="A8" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="30" t="s">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="32"/>
-      <c r="Z9" s="32"/>
-      <c r="AA9" s="33"/>
-      <c r="AB9" s="33"/>
-      <c r="AC9" s="33"/>
-      <c r="AD9" s="33"/>
-      <c r="AE9" s="33"/>
+      <c r="B9" s="4" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="35" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="B11" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="C11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="D11" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="E11" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="F11" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="36" t="s">
+      <c r="G11" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="38" t="s">
+      <c r="H11" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="38" t="s">
+      <c r="I11" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="M10" s="38" t="s">
+      <c r="J11" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="39" t="s">
+      <c r="M11" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="O10" s="38" t="s">
+      <c r="N11" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="P10" s="38" t="s">
+      <c r="O11" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="39" t="s">
+      <c r="P11" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="R10" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="S10" s="39" t="s">
+      <c r="Q11" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="R11" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="38" t="s">
+      <c r="S11" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="U10" s="38" t="s">
+      <c r="T11" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="V10" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="W10" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="X10" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y10" s="32"/>
-      <c r="Z10" s="32"/>
-      <c r="AA10" s="40"/>
-      <c r="AB10" s="40"/>
-      <c r="AC10" s="40"/>
-      <c r="AD10" s="40"/>
-      <c r="AE10" s="40"/>
+      <c r="U11" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="V11" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="W11" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="X11" s="33" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="L9:P9"/>
-    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="R10:U10"/>
+    <mergeCell ref="L10:Q10"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
- Making it workable
</commit_message>
<xml_diff>
--- a/src/main/resources/sample.xlsx
+++ b/src/main/resources/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stepway\smsa\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7CC35C-D0BE-483F-9C55-39B001B39CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CF4261-C448-4341-9EF4-4C6490CEFF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>Customer Name:</t>
   </si>
@@ -703,10 +703,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R1001"/>
+  <dimension ref="A1:U1001"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -726,9 +726,9 @@
     <col min="15" max="15" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -745,7 +745,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -762,7 +762,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -781,7 +781,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -800,7 +800,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -819,7 +819,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -838,7 +838,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -857,7 +857,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -879,9 +879,12 @@
         <v>7</v>
       </c>
       <c r="Q10" s="25"/>
-      <c r="R10" s="26"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="26"/>
     </row>
-    <row r="11" spans="1:18" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -933,11 +936,20 @@
       <c r="Q11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="R11" s="10" t="s">
+      <c r="R11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="T11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="U11" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -958,11 +970,14 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1950,7 +1965,7 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="P10:U10"/>
     <mergeCell ref="H10:N10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1965,7 +1980,7 @@
   </sheetPr>
   <dimension ref="A3:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- Added 3 New Columns and their Functionality in the Excel - Added 1 Column in the PDF but changes the values in the other columns as well.
</commit_message>
<xml_diff>
--- a/src/main/resources/sample.xlsx
+++ b/src/main/resources/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stepway\smsa\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CF4261-C448-4341-9EF4-4C6490CEFF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4727E89B-38C5-42DA-B29A-6CEB25F2BD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>Customer Name:</t>
   </si>
@@ -154,6 +154,21 @@
   </si>
   <si>
     <t>SMSA Admin Charges</t>
+  </si>
+  <si>
+    <t>VAT on SMSA Charges</t>
+  </si>
+  <si>
+    <t>Custom Declaration Currency</t>
+  </si>
+  <si>
+    <t>Charges as per Custom Declaration Currency</t>
+  </si>
+  <si>
+    <t>Custom Declaration#</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
   </si>
 </sst>
 </file>
@@ -703,10 +718,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U1001"/>
+  <dimension ref="A1:V1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -726,9 +741,9 @@
     <col min="15" max="15" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -745,7 +760,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -762,7 +777,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -781,7 +796,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -800,7 +815,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -819,7 +834,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -838,7 +853,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -857,7 +872,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -866,7 +881,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="27" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="I10" s="24"/>
       <c r="J10" s="25"/>
@@ -882,9 +897,10 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
-      <c r="U10" s="26"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="26"/>
     </row>
-    <row r="11" spans="1:21" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -901,7 +917,7 @@
         <v>12</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>14</v>
@@ -921,11 +937,11 @@
       <c r="L11" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="10" t="s">
+      <c r="M11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="O11" s="10" t="s">
         <v>17</v>
@@ -945,11 +961,14 @@
       <c r="T11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="U11" s="10" t="s">
-        <v>19</v>
+      <c r="U11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="V11" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -973,11 +992,12 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1965,11 +1985,12 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="P10:U10"/>
+    <mergeCell ref="P10:V10"/>
     <mergeCell ref="H10:N10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1978,10 +1999,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A3:AA11"/>
+  <dimension ref="A3:X11"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1991,15 +2012,15 @@
     <col min="14" max="14" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2007,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -2015,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -2023,7 +2044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -2031,7 +2052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -2039,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="13"/>
@@ -2064,15 +2085,12 @@
       </c>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="26"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="15"/>
+      <c r="U10" s="26"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
     </row>
-    <row r="11" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>24</v>
       </c>
@@ -2133,31 +2151,22 @@
       <c r="T11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="U11" s="22" t="s">
-        <v>37</v>
+      <c r="U11" s="21" t="s">
+        <v>19</v>
       </c>
       <c r="V11" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="W11" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="X11" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y11" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="Z11" s="21" t="s">
+      <c r="W11" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="AA11" s="22" t="s">
+      <c r="X11" s="22" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="R10:X10"/>
+    <mergeCell ref="R10:U10"/>
     <mergeCell ref="L10:Q10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Total Charges Fixed - Sample Updated
</commit_message>
<xml_diff>
--- a/src/main/resources/sample.xlsx
+++ b/src/main/resources/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stepway\smsa\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4727E89B-38C5-42DA-B29A-6CEB25F2BD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F79E25-9F7E-4F2B-B27E-A9B2F5537749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>Customer Name:</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Total Amount</t>
+  </si>
+  <si>
+    <t>Custom Declaration Date</t>
   </si>
 </sst>
 </file>
@@ -721,7 +724,7 @@
   <dimension ref="A1:V1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -908,7 +911,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>11</v>

</xml_diff>